<commit_message>
speed limiter / settings save / current calibration
</commit_message>
<xml_diff>
--- a/MINIMO.xlsx
+++ b/MINIMO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="28800" windowHeight="13620"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="28800" windowHeight="13620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CONTRL_TO_LCD data" sheetId="1" r:id="rId1"/>
@@ -1285,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU506"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S156" sqref="S156"/>
     </sheetView>
@@ -57327,7 +57327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
@@ -60873,7 +60873,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>